<commit_message>
Lernjournal added new times, correct some diagramms and slightly ediddts on java classes (persistence)
</commit_message>
<xml_diff>
--- a/2_Semester/aufgabe_3_team_3+4_lernjournal.xlsx
+++ b/2_Semester/aufgabe_3_team_3+4_lernjournal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26860" windowHeight="18140" tabRatio="415"/>
+    <workbookView xWindow="39320" yWindow="1100" windowWidth="26860" windowHeight="18140" tabRatio="415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lernjournal Aufgabe 3" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="39">
   <si>
     <t>Anleitung zum Lernjournal:</t>
   </si>
@@ -139,6 +139,27 @@
   </si>
   <si>
     <t>Dokumente ergeänzt und für Abgabe vorbereitet.</t>
+  </si>
+  <si>
+    <t>1.11.13</t>
+  </si>
+  <si>
+    <t>Erstellen erster Entwürfe für die Diagramme (Klassendiagram, 3-Schichten Paketdiagram und Sequenzdiagram)</t>
+  </si>
+  <si>
+    <t>Glossar Übersetzt</t>
+  </si>
+  <si>
+    <t>9.11.13</t>
+  </si>
+  <si>
+    <t>Diagramme besprochen und Angepasst.</t>
+  </si>
+  <si>
+    <t>Dokument für Aufgabe 4 vorbereitet</t>
+  </si>
+  <si>
+    <t>30.11.13</t>
   </si>
 </sst>
 </file>
@@ -317,8 +338,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -533,29 +558,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="105">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -606,6 +631,8 @@
     <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -656,6 +683,8 @@
     <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -987,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -1018,11 +1047,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1386,13 +1415,13 @@
       <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="39">
         <v>45</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="40">
         <v>41545</v>
       </c>
       <c r="D19" s="10"/>
@@ -1410,13 +1439,13 @@
       <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16" s="11" customFormat="1" ht="13" thickTop="1">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="43">
+      <c r="B20" s="42">
         <v>30</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="43">
         <v>41552</v>
       </c>
       <c r="D20" s="10"/>
@@ -1878,13 +1907,13 @@
       <c r="P40" s="10"/>
     </row>
     <row r="41" spans="1:16" s="11" customFormat="1" ht="25" thickBot="1">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="40">
+      <c r="B41" s="39">
         <v>45</v>
       </c>
-      <c r="C41" s="41">
+      <c r="C41" s="40">
         <v>41545</v>
       </c>
       <c r="D41" s="10"/>
@@ -2251,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="A24:C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2282,11 +2311,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2457,10 +2486,16 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
+    <row r="11" spans="1:16" s="11" customFormat="1">
+      <c r="A11" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="28">
+        <v>60</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -2571,11 +2606,11 @@
       </c>
       <c r="B17" s="18">
         <f>SUM(B11:B16)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C17" s="19">
         <f>TIME(0,B17,)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2709,10 +2744,16 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="30"/>
+    <row r="24" spans="1:16" s="11" customFormat="1">
+      <c r="A24" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="28">
+        <v>20</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>38</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -2727,10 +2768,16 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="1:16" s="11" customFormat="1">
-      <c r="A25" s="25"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="30"/>
+    <row r="25" spans="1:16" s="11" customFormat="1" ht="24">
+      <c r="A25" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="28">
+        <v>90</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -2745,10 +2792,16 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A26" s="25"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="30"/>
+    <row r="26" spans="1:16" s="11" customFormat="1">
+      <c r="A26" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="28">
+        <v>20</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -2764,9 +2817,15 @@
       <c r="P26" s="10"/>
     </row>
     <row r="27" spans="1:16" s="11" customFormat="1">
-      <c r="A27" s="25"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="30"/>
+      <c r="A27" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="28">
+        <v>60</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>35</v>
+      </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -2877,11 +2936,11 @@
       </c>
       <c r="B33" s="18">
         <f>SUM(B24:B32)</f>
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="C33" s="19">
         <f>TIME(0,B33,)</f>
-        <v>0</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -3110,11 +3169,11 @@
       </c>
       <c r="B45" s="16">
         <f>SUM(B33,B17)</f>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C45" s="17">
         <f>TIME(0,B45,)</f>
-        <v>0</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -3186,11 +3245,11 @@
       <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="60" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>

</xml_diff>